<commit_message>
Updated dashboard to include financials
</commit_message>
<xml_diff>
--- a/Dashboard.xlsx
+++ b/Dashboard.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26B0F0C-AFC5-AE4F-B830-4ED479AD6DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7979484-9749-7240-80D9-74B89F26D5BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{4F32CD4D-3FFC-624F-98AE-4C7FEFAF5D49}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{4F32CD4D-3FFC-624F-98AE-4C7FEFAF5D49}"/>
   </bookViews>
   <sheets>
     <sheet name="Big Tech" sheetId="1" r:id="rId1"/>
     <sheet name="Software" sheetId="4" r:id="rId2"/>
+    <sheet name="Financials" sheetId="5" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
@@ -43,6 +43,16 @@
     <externalReference r:id="rId26"/>
     <externalReference r:id="rId27"/>
     <externalReference r:id="rId28"/>
+    <externalReference r:id="rId29"/>
+    <externalReference r:id="rId30"/>
+    <externalReference r:id="rId31"/>
+    <externalReference r:id="rId32"/>
+    <externalReference r:id="rId33"/>
+    <externalReference r:id="rId34"/>
+    <externalReference r:id="rId35"/>
+    <externalReference r:id="rId36"/>
+    <externalReference r:id="rId37"/>
+    <externalReference r:id="rId38"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -69,7 +79,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="26">
+  <futureMetadata name="XLRICHVALUE" count="35">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -252,8 +262,71 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="91"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="94"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="97"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="100"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="103"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="106"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="109"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="112"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="115"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="26">
+  <valueMetadata count="35">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -332,12 +405,39 @@
     <bk>
       <rc t="1" v="25"/>
     </bk>
+    <bk>
+      <rc t="1" v="26"/>
+    </bk>
+    <bk>
+      <rc t="1" v="27"/>
+    </bk>
+    <bk>
+      <rc t="1" v="28"/>
+    </bk>
+    <bk>
+      <rc t="1" v="29"/>
+    </bk>
+    <bk>
+      <rc t="1" v="30"/>
+    </bk>
+    <bk>
+      <rc t="1" v="31"/>
+    </bk>
+    <bk>
+      <rc t="1" v="32"/>
+    </bk>
+    <bk>
+      <rc t="1" v="33"/>
+    </bk>
+    <bk>
+      <rc t="1" v="34"/>
+    </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="12">
   <si>
     <t>Big Tech</t>
   </si>
@@ -1648,6 +1748,186 @@
 </externalLink>
 </file>
 
+<file path=xl/externalLinks/externalLink27.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet 1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="4">
+          <cell r="AJ4">
+            <v>-0.14817164642055514</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="AP7" t="str">
+            <v>- -</v>
+          </cell>
+          <cell r="AS7">
+            <v>7.2031752231958138E-2</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="AR13">
+            <v>-5.3649750927818686E-2</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="AQ16">
+            <v>2.2769253431935623</v>
+          </cell>
+          <cell r="AR16">
+            <v>-30.143043078136639</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="AJ20">
+            <v>-1.0176404064859355</v>
+          </cell>
+        </row>
+        <row r="101">
+          <cell r="AR101">
+            <v>687834100000</v>
+          </cell>
+        </row>
+        <row r="115">
+          <cell r="AL115">
+            <v>338.34949429784706</v>
+          </cell>
+        </row>
+        <row r="117">
+          <cell r="AL117">
+            <v>8.2683735873562592E-2</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink28.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet 1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="4">
+          <cell r="Z4">
+            <v>-7.7474966449881277E-2</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="AF7">
+            <v>0.49159999999999998</v>
+          </cell>
+          <cell r="AI7">
+            <v>0.24746824819560231</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="AH13">
+            <v>0.13786143746414839</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="AG16">
+            <v>5.5175493761539753</v>
+          </cell>
+          <cell r="AH16">
+            <v>19.04502896871379</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="Z20">
+            <v>-0.19460478265991288</v>
+          </cell>
+        </row>
+        <row r="100">
+          <cell r="AH100">
+            <v>98615160000</v>
+          </cell>
+        </row>
+        <row r="115">
+          <cell r="AB115">
+            <v>593.13941771467114</v>
+          </cell>
+        </row>
+        <row r="117">
+          <cell r="AB117">
+            <v>-9.6375049185449146E-2</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink29.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet 1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="4">
+          <cell r="X4">
+            <v>7.0303004456575113E-2</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="AD7">
+            <v>0.85</v>
+          </cell>
+          <cell r="AG7">
+            <v>0.60883770968641671</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="AF13">
+            <v>9.9478512126819518E-2</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="AE16">
+            <v>13.982792764075388</v>
+          </cell>
+          <cell r="AF16">
+            <v>26.081467855815681</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="X20">
+            <v>2.2978549956692351E-2</v>
+          </cell>
+        </row>
+        <row r="101">
+          <cell r="AF101">
+            <v>70185230000</v>
+          </cell>
+        </row>
+        <row r="115">
+          <cell r="Z115">
+            <v>277.02893053430296</v>
+          </cell>
+        </row>
+        <row r="117">
+          <cell r="Z117">
+            <v>0.41623092139616036</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -1698,6 +1978,366 @@
         <row r="117">
           <cell r="Z117">
             <v>-6.8556062352238545E-3</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink30.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet 1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="4">
+          <cell r="AB4">
+            <v>0.15862753660981066</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="AH7">
+            <v>0.52759999999999996</v>
+          </cell>
+          <cell r="AK7">
+            <v>0.26418087393404821</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="AJ13">
+            <v>0.13387678195897726</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="AI16">
+            <v>8.4120761953520056</v>
+          </cell>
+          <cell r="AJ16">
+            <v>39.078598296369265</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="AB20">
+            <v>3.6980525791585839E-2</v>
+          </cell>
+        </row>
+        <row r="101">
+          <cell r="AJ101">
+            <v>15510960000</v>
+          </cell>
+        </row>
+        <row r="115">
+          <cell r="AD115">
+            <v>338.60998990983916</v>
+          </cell>
+        </row>
+        <row r="117">
+          <cell r="AD117">
+            <v>-0.16347154031859479</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink31.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet 1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="4">
+          <cell r="AL4">
+            <v>4.6131666737559751E-2</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="AR7">
+            <v>0.78059999999999996</v>
+          </cell>
+          <cell r="AU7">
+            <v>0.36552092182360757</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="AT13">
+            <v>0.48853670640728536</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="AS16">
+            <v>12.2812302598619</v>
+          </cell>
+          <cell r="AT16">
+            <v>45.281695985179674</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="AL20">
+            <v>4.0671756745220167E-2</v>
+          </cell>
+        </row>
+        <row r="101">
+          <cell r="AT101">
+            <v>16914570000</v>
+          </cell>
+        </row>
+        <row r="115">
+          <cell r="AN115">
+            <v>363.64699332556165</v>
+          </cell>
+        </row>
+        <row r="117">
+          <cell r="AN117">
+            <v>-0.45919664298271667</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink32.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet 1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="4">
+          <cell r="AA4">
+            <v>-0.12061756191701511</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="AG7">
+            <v>0.70499999999999996</v>
+          </cell>
+          <cell r="AJ7">
+            <v>0.26956839795171911</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="AI13">
+            <v>0.18137160470044308</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="AH16">
+            <v>10.00873811265545</v>
+          </cell>
+          <cell r="AI16">
+            <v>39.83098981077147</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="AA20">
+            <v>-0.41394335511982572</v>
+          </cell>
+        </row>
+        <row r="101">
+          <cell r="AI101">
+            <v>54727780000</v>
+          </cell>
+        </row>
+        <row r="115">
+          <cell r="AC115">
+            <v>137.33486258013255</v>
+          </cell>
+        </row>
+        <row r="117">
+          <cell r="AC117">
+            <v>-0.54010159205635078</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink33.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet 1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="4">
+          <cell r="U4">
+            <v>0.10034234643345097</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="AA7">
+            <v>0.77969999999999995</v>
+          </cell>
+          <cell r="AD7">
+            <v>0.48107843198295114</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="AC13">
+            <v>0.33217112132371146</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="AB16">
+            <v>19.001008628487618</v>
+          </cell>
+          <cell r="AC16">
+            <v>49.077596020092514</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="U20">
+            <v>0.15552034725990227</v>
+          </cell>
+        </row>
+        <row r="101">
+          <cell r="AC101">
+            <v>42725630000</v>
+          </cell>
+        </row>
+        <row r="115">
+          <cell r="W115">
+            <v>304.30091676100784</v>
+          </cell>
+        </row>
+        <row r="117">
+          <cell r="W117">
+            <v>-0.42977435255128293</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink34.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet 1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="4">
+          <cell r="AM4">
+            <v>0.34759551645172948</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="AS7">
+            <v>0.66320000000000001</v>
+          </cell>
+          <cell r="AV7">
+            <v>0.22484572041856721</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="AU13">
+            <v>6.2882732764007493E-2</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="AT16">
+            <v>9.9976925140863973</v>
+          </cell>
+          <cell r="AU16">
+            <v>34.416317733990148</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="AM20">
+            <v>0.36072951207958304</v>
+          </cell>
+        </row>
+        <row r="101">
+          <cell r="AU101">
+            <v>111784200000</v>
+          </cell>
+        </row>
+        <row r="115">
+          <cell r="AO115">
+            <v>114.61927965594801</v>
+          </cell>
+        </row>
+        <row r="117">
+          <cell r="AO117">
+            <v>-0.66373502418603536</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink35.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet 1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="4">
+          <cell r="T4">
+            <v>0.21593030491599263</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="Z7">
+            <v>0.8044</v>
+          </cell>
+          <cell r="AC7">
+            <v>0.60999658819515523</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="AB13">
+            <v>0.32418879564370767</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="AA16">
+            <v>15.869447287615149</v>
+          </cell>
+          <cell r="AB16">
+            <v>31.098047736845626</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="T20">
+            <v>0.12399309551208293</v>
+          </cell>
+        </row>
+        <row r="101">
+          <cell r="AB101">
+            <v>465133500000</v>
+          </cell>
+        </row>
+        <row r="115">
+          <cell r="V115">
+            <v>243.16631410410545</v>
+          </cell>
+        </row>
+        <row r="117">
+          <cell r="V117">
+            <v>7.6004752883337412E-2</v>
           </cell>
         </row>
       </sheetData>
@@ -2164,7 +2804,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="89">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="116">
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a24kar&amp;q=XNAS%3aTSLA&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
@@ -3618,11 +4258,494 @@
   <rv s="2">
     <v>87</v>
   </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a23d9c&amp;q=XNYS%3aSPGI&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>0</v>
+    <v>S&amp;P Global Inc. (XNYS:SPGI)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>en-US</v>
+    <v>a23d9c</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>416.36</v>
+    <v>279.32</v>
+    <v>1.1156999999999999</v>
+    <v>-3.74</v>
+    <v>-1.0853E-2</v>
+    <v>2.34</v>
+    <v>6.8649999999999996E-3</v>
+    <v>USD</v>
+    <v>S&amp;P Global Inc. is a provider of credit ratings, benchmarks, analytics and workflow solutions in the global capital, commodity and automotive markets. It comprises six operating divisions: S&amp;P Global Market Intelligence (Market Intelligence), S&amp;P Global Ratings (Ratings), S&amp;P Global Commodity Insights (Commodity Insights), S&amp;P Global Mobility (Mobility), S&amp;P Dow Jones Indices (Indices), and S&amp;P Global Engineering Solutions (Engineering Solutions). Its Market Intelligence business lines include desktop, data &amp; advisory solutions, enterprise solutions and credit risk solutions. Its Ratings provides credit ratings, research and analytics to investors and other market participants. Its Commodity Insights is an independent provider of information and benchmark prices for the commodity and energy markets. Its Mobility provides insights, forecasts and advisory services to automotive value chain. Its Indices is an index provider that maintains a range of indices to meet various investor needs.</v>
+    <v>39950</v>
+    <v>New York Stock Exchange</v>
+    <v>XNYS</v>
+    <v>XNYS</v>
+    <v>55 Water St, NEW YORK, NY, 10041-0004 US</v>
+    <v>343.4</v>
+    <v>Professional &amp; Commercial Services</v>
+    <v>Stock</v>
+    <v>45022.982271712499</v>
+    <v>89</v>
+    <v>334.5</v>
+    <v>111784200000</v>
+    <v>S&amp;P Global Inc.</v>
+    <v>S&amp;P Global Inc.</v>
+    <v>343.4</v>
+    <v>32.830100000000002</v>
+    <v>344.6</v>
+    <v>340.86</v>
+    <v>343.2</v>
+    <v>327947400</v>
+    <v>SPGI</v>
+    <v>S&amp;P Global Inc. (XNYS:SPGI)</v>
+    <v>1309958</v>
+    <v>1496609</v>
+    <v>1925</v>
+  </rv>
+  <rv s="2">
+    <v>90</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a256cw&amp;q=XNYS%3aV&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>0</v>
+    <v>VISA INC. (XNYS:V)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>en-US</v>
+    <v>a256cw</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>234.3</v>
+    <v>174.6</v>
+    <v>0.9647</v>
+    <v>-2.1800000000000002</v>
+    <v>-9.554E-3</v>
+    <v>0</v>
+    <v>0</v>
+    <v>USD</v>
+    <v>Visa Inc. (Visa) is a global payments technology company. The Company provides digital payments across more than 200 countries and territories. The Company connects consumers, merchants, financial institutions, businesses, strategic partners and government entities through technologies. The Company operates through the payment services segment. The Company provides transaction processing services, including primarily authorization, clearing and settlement to its financial institution and merchant clients through VisaNet, its transaction processing network. Its core business solutions, including credit, debit, prepaid and cash access programs for individual, business and government account holders. It also provides value-added services to its clients, including issuing solutions, acceptance solutions, risk and identity solutions, open banking and advisory services. It also offers products and solutions that facilitate money movement for all participants in the ecosystem.</v>
+    <v>26500</v>
+    <v>New York Stock Exchange</v>
+    <v>XNYS</v>
+    <v>XNYS</v>
+    <v>P.O. Box 8999, SAN FRANCISCO, CA, 94128-8999 US</v>
+    <v>226.73</v>
+    <v>Software &amp; IT Services</v>
+    <v>Stock</v>
+    <v>45022.999148460156</v>
+    <v>92</v>
+    <v>224.68</v>
+    <v>465133500000</v>
+    <v>VISA INC.</v>
+    <v>VISA INC.</v>
+    <v>226.16</v>
+    <v>31.911899999999999</v>
+    <v>228.17</v>
+    <v>225.99</v>
+    <v>225.99</v>
+    <v>2058204000</v>
+    <v>V</v>
+    <v>VISA INC. (XNYS:V)</v>
+    <v>4285206</v>
+    <v>7178888</v>
+    <v>2007</v>
+  </rv>
+  <rv s="2">
+    <v>93</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1sqcw&amp;q=XNYS%3aFDS&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>0</v>
+    <v>FACTSET RESEARCH SYSTEMS INC. (XNYS:FDS)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>en-US</v>
+    <v>a1sqcw</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>474.13</v>
+    <v>345.92</v>
+    <v>0.82889999999999997</v>
+    <v>2.74</v>
+    <v>6.8149999999999999E-3</v>
+    <v>4.45</v>
+    <v>1.0993999999999999E-2</v>
+    <v>USD</v>
+    <v>FactSet Research Systems Inc. is a global financial data and analytics company. The Company provides financial data and market intelligence on securities, companies and industries to enable its clients to research investment ideas, as well as offering them the capabilities to analyze, monitor and manage their portfolios. The Company also offers technologies, such as a configurable desktop and mobile platform, comprehensive data feeds, cloud-based digital solutions, and application programming interfaces (APIs). Its solutions span investment research, portfolio construction and analysis, trade execution, performance measurement, risk management, and reporting across the investment lifecycle. The Company operates through three geographical segments: the Americas, EMEA and Asia Pacific. It primarily delivers insight and information through its three workflow solutions: Research &amp; Advisory; Analytics &amp; Trading; and Content &amp; Technology (CTS).</v>
+    <v>11896</v>
+    <v>New York Stock Exchange</v>
+    <v>XNYS</v>
+    <v>XNYS</v>
+    <v>45 Glover Avenue, NORWALK, CT, 06850 US</v>
+    <v>405.66</v>
+    <v>Professional &amp; Commercial Services</v>
+    <v>Stock</v>
+    <v>45022.958333356248</v>
+    <v>95</v>
+    <v>399.74</v>
+    <v>15510960000</v>
+    <v>FACTSET RESEARCH SYSTEMS INC.</v>
+    <v>FACTSET RESEARCH SYSTEMS INC.</v>
+    <v>400.6</v>
+    <v>34.9754</v>
+    <v>402.04</v>
+    <v>404.78</v>
+    <v>409.23</v>
+    <v>38319490</v>
+    <v>FDS</v>
+    <v>FACTSET RESEARCH SYSTEMS INC. (XNYS:FDS)</v>
+    <v>205113</v>
+    <v>316827</v>
+    <v>1984</v>
+  </rv>
+  <rv s="2">
+    <v>96</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1xz1h&amp;q=XNYS%3aMSCI&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>0</v>
+    <v>MSCI INC. (XNYS:MSCI)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>en-US</v>
+    <v>a1xz1h</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>572.5</v>
+    <v>376.41</v>
+    <v>1.1511</v>
+    <v>-4.72</v>
+    <v>-8.7670000000000005E-3</v>
+    <v>0</v>
+    <v>0</v>
+    <v>USD</v>
+    <v>MSCI Inc. (MSCI) is a provider of critical decision support tools and solutions for the global investment community. The Company operates through four segments: Index, Analytics, ESG and Climate, and All Other-Private Assets. Its Index segment offers products, such as MSCI Global Equity Indexes, ESG and Climate Indexes, Factor Indexes, Thematic Indexes, Custom Indexes, Fixed Income Indexes and Real Estate Indexes. Its Analytics segment offers risk management, performance attribution and portfolio management content, applications and services. Its ESG and Climate segment offerings include MSCI ESG Ratings, MSCI ESG Business Involvement Screening Research, and MSCI Climate Solutions. Its All Other-Private Assets segment comprises the Real Estate and Burgiss segments. The Real Estate segment offerings include offerings include transaction data, benchmarks, return-analytics, climate assessments and market insights for tangible assets, such as real estate and infrastructure.</v>
+    <v>4759</v>
+    <v>New York Stock Exchange</v>
+    <v>XNYS</v>
+    <v>XNYS</v>
+    <v>250 Greenwich Street, 49Th Floor, 7 World Trade Center, NEW YORK, NY, 10007 US</v>
+    <v>537.39</v>
+    <v>Professional &amp; Commercial Services</v>
+    <v>Stock</v>
+    <v>45022.958333356248</v>
+    <v>98</v>
+    <v>532.36</v>
+    <v>42725630000</v>
+    <v>MSCI INC.</v>
+    <v>MSCI INC.</v>
+    <v>534.21</v>
+    <v>50.2318</v>
+    <v>538.37</v>
+    <v>533.65</v>
+    <v>533.65</v>
+    <v>80063020</v>
+    <v>MSCI</v>
+    <v>MSCI INC. (XNYS:MSCI)</v>
+    <v>333499</v>
+    <v>447745</v>
+    <v>1998</v>
+  </rv>
+  <rv s="2">
+    <v>99</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1px2w&amp;q=XNAS%3aCME&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>0</v>
+    <v>CME GROUP INC. (XNAS:CME)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>en-US</v>
+    <v>a1px2w</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>240.602</v>
+    <v>162.25530000000001</v>
+    <v>0.41620000000000001</v>
+    <v>-0.09</v>
+    <v>-4.6109999999999999E-4</v>
+    <v>0.51</v>
+    <v>2.614E-3</v>
+    <v>USD</v>
+    <v>CME Group Inc. provides products across all asset classes, by trading futures, options, cash and over-the-counter (OTC) products. The Company offers a range of interest rates, equity indexes, foreign exchange (FX), agricultural commodities, energy and metals. It also offers cash and repo fixed income trading through BrokerTec, and cash and OTC FX trading through electronic broking services (EBS). The Company’s operations comprise of the businesses of Chicago Mercantile Exchange Inc. (CME), the Board of Trade of the City of Chicago, Inc. (CBOT), New York Mercantile Exchange, Inc. (NYMEX) and Commodity Exchange, Inc. (COMEX) and its cash markets business. In addition, it operates central counterparty clearing houses. The Company offers clearing, settlement and guarantees for all products cleared through the clearing house. It provides clearing and settlement services for a range of exchange-traded futures and options on futures contracts and OTC derivatives.</v>
+    <v>3460</v>
+    <v>Nasdaq Stock Market</v>
+    <v>XNAS</v>
+    <v>XNAS</v>
+    <v>20 S Wacker Dr, CHICAGO, IL, 60606 US</v>
+    <v>196.3</v>
+    <v>Investment Banking &amp; Investment Services</v>
+    <v>Stock</v>
+    <v>45022.978680601562</v>
+    <v>101</v>
+    <v>193.78</v>
+    <v>70185230000</v>
+    <v>CME GROUP INC.</v>
+    <v>CME GROUP INC.</v>
+    <v>195.3</v>
+    <v>26.401299999999999</v>
+    <v>195.19</v>
+    <v>195.1</v>
+    <v>195.61</v>
+    <v>359739700</v>
+    <v>CME</v>
+    <v>CME GROUP INC. (XNAS:CME)</v>
+    <v>1370087</v>
+    <v>1985947</v>
+    <v>2001</v>
+  </rv>
+  <rv s="2">
+    <v>102</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1svnm&amp;q=XNYS%3aFICO&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>0</v>
+    <v>FAIR ISAAC CORPORATION (XNYS:FICO)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>en-US</v>
+    <v>a1svnm</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>711.84500000000003</v>
+    <v>340.48</v>
+    <v>1.2672000000000001</v>
+    <v>-4.2</v>
+    <v>-6.2070000000000007E-3</v>
+    <v>0</v>
+    <v>0</v>
+    <v>USD</v>
+    <v>Fair Isaac Corporation is an applied analytics company. The Company operates through two segments: Scores and Software. The Scores segment includes its business-to-business (B2B) scoring solutions and services which give its clients access to predictive credit and other scores that can be integrated into their transaction streams and decision-making processes. This segment also includes its business-to-consumer (B2C) scoring solutions, including its myFICO.com subscription offerings. The Software segment includes pre-configured analytic and decision management solutions designed for a specific type of business need or process, such as account origination, customer management, customer engagement, fraud detection, financial crimes compliance and marketing as well as associated professional services. This segment also includes FICO Platform, a modular software offering designed to support advanced analytic and decision use cases, as well as stand-alone analytic and decisioning software.</v>
+    <v>3305</v>
+    <v>New York Stock Exchange</v>
+    <v>XNYS</v>
+    <v>XNYS</v>
+    <v>5 West Mendenhall, Suites 105, BOZEMAN, MT, 59715 US</v>
+    <v>677</v>
+    <v>Software &amp; IT Services</v>
+    <v>Stock</v>
+    <v>45022.958333367969</v>
+    <v>104</v>
+    <v>668.98</v>
+    <v>16914570000</v>
+    <v>FAIR ISAAC CORPORATION</v>
+    <v>FAIR ISAAC CORPORATION</v>
+    <v>671.3</v>
+    <v>45.255699999999997</v>
+    <v>676.62</v>
+    <v>672.42</v>
+    <v>672.42</v>
+    <v>25154780</v>
+    <v>FICO</v>
+    <v>FAIR ISAAC CORPORATION (XNYS:FICO)</v>
+    <v>127596</v>
+    <v>432187</v>
+    <v>1987</v>
+  </rv>
+  <rv s="2">
+    <v>105</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1om4c&amp;q=XNYS%3aBLK&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>0</v>
+    <v>BLACKROCK, INC. (XNYS:BLK)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>en-US</v>
+    <v>a1om4c</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>785.65</v>
+    <v>503.12360000000001</v>
+    <v>1.2902</v>
+    <v>0.36</v>
+    <v>5.4870000000000006E-4</v>
+    <v>-0.1</v>
+    <v>-1.5230000000000002E-4</v>
+    <v>USD</v>
+    <v>BlackRock, Inc. is an investment management company. The Company provides a range of investment management and technology services to institutional and retail clients. Its diverse platform of alpha-seeking active, index and cash management investment strategies across asset classes enables the Company to tailor investment outcomes and asset allocation solutions for clients. The Company's product offerings include single- and multi-asset portfolios investing in equities, fixed income, alternatives and money market instruments. Its products are offered directly and through intermediaries in a range of vehicles, including open-end and closed-end mutual funds, iShares exchange-traded funds (ETFs), separate accounts, collective investment funds and other pooled investment vehicles. The Company also offers technology services, including the investment and risk management technology platform, Aladdin, Aladdin Wealth, eFront, and Cachematrix, as well as advisory services and solutions.</v>
+    <v>19800</v>
+    <v>New York Stock Exchange</v>
+    <v>XNYS</v>
+    <v>XNYS</v>
+    <v>50 Hudson Yards, NEW YORK, NY, 10001 US</v>
+    <v>659.06</v>
+    <v>Investment Banking &amp; Investment Services</v>
+    <v>Stock</v>
+    <v>45022.991158888282</v>
+    <v>107</v>
+    <v>653.98500000000001</v>
+    <v>98615160000</v>
+    <v>BLACKROCK, INC.</v>
+    <v>BLACKROCK, INC.</v>
+    <v>656.6</v>
+    <v>19.322199999999999</v>
+    <v>656.04</v>
+    <v>656.4</v>
+    <v>656.3</v>
+    <v>150236400</v>
+    <v>BLK</v>
+    <v>BLACKROCK, INC. (XNYS:BLK)</v>
+    <v>441769</v>
+    <v>726414</v>
+    <v>2006</v>
+  </rv>
+  <rv s="2">
+    <v>108</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1xear&amp;q=XNYS%3aMCO&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>0</v>
+    <v>MOODY'S CORPORATION (XNYS:MCO)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>en-US</v>
+    <v>a1xear</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>346.22</v>
+    <v>230.16</v>
+    <v>1.2968999999999999</v>
+    <v>-4.2300000000000004</v>
+    <v>-1.3967E-2</v>
+    <v>0</v>
+    <v>0</v>
+    <v>USD</v>
+    <v>Moody's Corporation is a global integrated risk assessment company. The Company operates through two segments: Moody's Investors Service (MIS), and Moody's Analytics (MA). The MIS segment publishes credit ratings and provides assessment services on a range of debt obligations, programs and facilities, and the entities that issue such obligations in markets worldwide, including various corporate, financial institution and governmental obligations, and structured finance securities. The MIS segment consists of five lines of business, which include corporate finance group; structured finance group; financial institutions group; public, project and infrastructure finance, and MIS Other. The MA segment develops a range of products and services that support the risk management activities of institutional participants in global financial markets. The MA segment consists of three lines of business, such as decision solutions, research and insights, and data and information.</v>
+    <v>14426</v>
+    <v>New York Stock Exchange</v>
+    <v>XNYS</v>
+    <v>XNYS</v>
+    <v>7 World Trade Ctr, NEW YORK, NY, 10007-2140 US</v>
+    <v>302.83999999999997</v>
+    <v>Professional &amp; Commercial Services</v>
+    <v>Stock</v>
+    <v>45022.958333344533</v>
+    <v>110</v>
+    <v>296.16000000000003</v>
+    <v>54727780000</v>
+    <v>MOODY'S CORPORATION</v>
+    <v>MOODY'S CORPORATION</v>
+    <v>302.02</v>
+    <v>39.387</v>
+    <v>302.85000000000002</v>
+    <v>298.62</v>
+    <v>298.62</v>
+    <v>183269000</v>
+    <v>MCO</v>
+    <v>MOODY'S CORPORATION (XNYS:MCO)</v>
+    <v>564454</v>
+    <v>837019</v>
+    <v>2000</v>
+  </rv>
+  <rv s="2">
+    <v>111</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1otp2&amp;q=XNYS%3aBRK.A&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="8">
+    <v>14</v>
+    <v>BERKSHIRE HATHAWAY INC., (XNYS:BRK.A)</v>
+    <v>2</v>
+    <v>15</v>
+    <v>Finance</v>
+    <v>16</v>
+    <v>en-US</v>
+    <v>a1otp2</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>531880</v>
+    <v>393012.25</v>
+    <v>0.87180000000000002</v>
+    <v>6505</v>
+    <v>1.3795999999999999E-2</v>
+    <v>USD</v>
+    <v>Berkshire Hathaway Inc. (Berkshire) is a holding company owning subsidiaries engaged in various business activities. Berkshire’s various business activities include insurance businesses conducted on both a primary basis and a reinsurance basis. Its segments include Insurance, which consists of GEICO, Berkshire Hathaway Primary Group and Berkshire Hathaway Reinsurance Group; Railroad, which includes operations of railroad systems in North America through Burlington Northern Santa Fe LLC; Utilities and energy, which includes regulated electric and gas utility; Manufacturing, which include manufacture of various products, including industrial, consumer and building products; McLane Company, which include wholesale distribution of groceries and non-food items, and Service and retailing, which provide shared aircraft ownership programs, aviation pilot training, electronic components distribution and various retailing businesses, including automobile dealerships and furniture leasing.</v>
+    <v>383000</v>
+    <v>New York Stock Exchange</v>
+    <v>XNYS</v>
+    <v>XNYS</v>
+    <v>3555 Farnam St, OMAHA, NE, 68131 US</v>
+    <v>478580.98879999999</v>
+    <v>Consumer Goods Conglomerates</v>
+    <v>Stock</v>
+    <v>45022.958333356248</v>
+    <v>113</v>
+    <v>467601.01</v>
+    <v>687834100000</v>
+    <v>BERKSHIRE HATHAWAY INC.,</v>
+    <v>BERKSHIRE HATHAWAY INC.,</v>
+    <v>473479.44880000001</v>
+    <v>58.279499999999999</v>
+    <v>471500</v>
+    <v>478005</v>
+    <v>1455700</v>
+    <v>BRK.A</v>
+    <v>BERKSHIRE HATHAWAY INC., (XNYS:BRK.A)</v>
+    <v>5095</v>
+    <v>4769</v>
+    <v>1998</v>
+  </rv>
+  <rv s="2">
+    <v>114</v>
+  </rv>
 </rvData>
 </file>
 
 <file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="8">
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="9">
   <s t="_hyperlink">
     <k n="Address" t="s"/>
     <k n="Text" t="s"/>
@@ -3830,12 +4953,56 @@
     <k n="Volume average"/>
     <k n="Year incorporated"/>
   </s>
+  <s t="_linkedentitycore">
+    <k n="_Display" t="spb"/>
+    <k n="_DisplayString" t="s"/>
+    <k n="_Flags" t="spb"/>
+    <k n="_Format" t="spb"/>
+    <k n="_Icon" t="s"/>
+    <k n="_SubLabel" t="spb"/>
+    <k n="%EntityCulture" t="s"/>
+    <k n="%EntityId" t="s"/>
+    <k n="%EntityServiceId"/>
+    <k n="%IsRefreshable" t="b"/>
+    <k n="%ProviderInfo" t="s"/>
+    <k n="52 week high"/>
+    <k n="52 week low"/>
+    <k n="Beta"/>
+    <k n="Change"/>
+    <k n="Change (%)"/>
+    <k n="Currency" t="s"/>
+    <k n="Description" t="s"/>
+    <k n="Employees"/>
+    <k n="Exchange" t="s"/>
+    <k n="Exchange abbreviation" t="s"/>
+    <k n="ExchangeID" t="s"/>
+    <k n="Headquarters" t="s"/>
+    <k n="High"/>
+    <k n="Industry" t="s"/>
+    <k n="Instrument type" t="s"/>
+    <k n="Last trade time"/>
+    <k n="LearnMoreOnLink" t="r"/>
+    <k n="Low"/>
+    <k n="Market cap"/>
+    <k n="Name" t="s"/>
+    <k n="Official name" t="s"/>
+    <k n="Open"/>
+    <k n="P/E"/>
+    <k n="Previous close"/>
+    <k n="Price"/>
+    <k n="Shares outstanding"/>
+    <k n="Ticker symbol" t="s"/>
+    <k n="UniqueName" t="s"/>
+    <k n="Volume"/>
+    <k n="Volume average"/>
+    <k n="Year incorporated"/>
+  </s>
 </rvStructures>
 </file>
 
 <file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
 <supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
-  <spbArrays count="4">
+  <spbArrays count="5">
     <a count="45">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
@@ -4024,8 +5191,52 @@
       <v t="s">ExchangeID</v>
       <v t="s">%ProviderInfo</v>
     </a>
+    <a count="42">
+      <v t="s">%EntityServiceId</v>
+      <v t="s">_Format</v>
+      <v t="s">%IsRefreshable</v>
+      <v t="s">%EntityCulture</v>
+      <v t="s">%EntityId</v>
+      <v t="s">_Icon</v>
+      <v t="s">_Display</v>
+      <v t="s">Name</v>
+      <v t="s">_SubLabel</v>
+      <v t="s">Price</v>
+      <v t="s">Exchange</v>
+      <v t="s">Official name</v>
+      <v t="s">Last trade time</v>
+      <v t="s">Ticker symbol</v>
+      <v t="s">Exchange abbreviation</v>
+      <v t="s">Change</v>
+      <v t="s">Change (%)</v>
+      <v t="s">Currency</v>
+      <v t="s">Previous close</v>
+      <v t="s">Open</v>
+      <v t="s">High</v>
+      <v t="s">Low</v>
+      <v t="s">52 week high</v>
+      <v t="s">52 week low</v>
+      <v t="s">Volume</v>
+      <v t="s">Volume average</v>
+      <v t="s">Market cap</v>
+      <v t="s">Beta</v>
+      <v t="s">P/E</v>
+      <v t="s">Shares outstanding</v>
+      <v t="s">Description</v>
+      <v t="s">Employees</v>
+      <v t="s">Headquarters</v>
+      <v t="s">Industry</v>
+      <v t="s">Instrument type</v>
+      <v t="s">Year incorporated</v>
+      <v t="s">_Flags</v>
+      <v t="s">UniqueName</v>
+      <v t="s">_DisplayString</v>
+      <v t="s">LearnMoreOnLink</v>
+      <v t="s">ExchangeID</v>
+      <v t="s">%ProviderInfo</v>
+    </a>
   </spbArrays>
-  <spbData count="14">
+  <spbData count="17">
     <spb s="0">
       <v>0</v>
       <v>Name</v>
@@ -4181,12 +5392,46 @@
       <v>1</v>
       <v>5</v>
     </spb>
+    <spb s="0">
+      <v>4</v>
+      <v>Name</v>
+      <v>LearnMoreOnLink</v>
+    </spb>
+    <spb s="11">
+      <v>1</v>
+      <v>2</v>
+      <v>2</v>
+      <v>1</v>
+      <v>3</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>4</v>
+      <v>4</v>
+      <v>5</v>
+      <v>6</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>4</v>
+      <v>7</v>
+      <v>8</v>
+      <v>9</v>
+      <v>4</v>
+    </spb>
+    <spb s="12">
+      <v>Delayed 15 minutes</v>
+      <v>from previous close</v>
+      <v>from previous close</v>
+      <v>Source: Nasdaq</v>
+      <v>GMT</v>
+    </spb>
   </spbData>
 </supportingPropertyBags>
 </file>
 
 <file path=xl/richData/rdsupportingpropertybagstructure.xml><?xml version="1.0" encoding="utf-8"?>
-<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="11">
+<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="13">
   <s>
     <k n="^Order" t="spba"/>
     <k n="TitleProperty" t="s"/>
@@ -4326,6 +5571,35 @@
     <k n="Price (Extended hours)" t="i"/>
     <k n="Change (Extended hours)" t="i"/>
     <k n="Change % (Extended hours)" t="i"/>
+  </s>
+  <s>
+    <k n="Low" t="i"/>
+    <k n="P/E" t="i"/>
+    <k n="Beta" t="i"/>
+    <k n="High" t="i"/>
+    <k n="Name" t="i"/>
+    <k n="Open" t="i"/>
+    <k n="Price" t="i"/>
+    <k n="Change" t="i"/>
+    <k n="Volume" t="i"/>
+    <k n="Employees" t="i"/>
+    <k n="Change (%)" t="i"/>
+    <k n="Market cap" t="i"/>
+    <k n="52 week low" t="i"/>
+    <k n="52 week high" t="i"/>
+    <k n="Previous close" t="i"/>
+    <k n="Volume average" t="i"/>
+    <k n="Last trade time" t="i"/>
+    <k n="Year incorporated" t="i"/>
+    <k n="`%EntityServiceId" t="i"/>
+    <k n="Shares outstanding" t="i"/>
+  </s>
+  <s>
+    <k n="Price" t="s"/>
+    <k n="Change" t="s"/>
+    <k n="Change (%)" t="s"/>
+    <k n="ExchangeID" t="s"/>
+    <k n="Last trade time" t="s"/>
   </s>
 </spbStructures>
 </file>
@@ -4690,9 +5964,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{238F2BC1-9023-1247-98E3-2B9EA07C7262}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N8" sqref="N8"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5235,8 +6509,8 @@
       <c r="K18" s="8"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G16">
-    <sortCondition descending="1" ref="D1:D16"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K18">
+    <sortCondition descending="1" ref="D1:D18"/>
   </sortState>
   <conditionalFormatting sqref="C2:C10 D10:E10">
     <cfRule type="colorScale" priority="17">
@@ -5387,7 +6661,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C18"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5395,7 +6669,11 @@
     <col min="1" max="1" width="32.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
-    <col min="4" max="10" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" hidden="1" customWidth="1"/>
+    <col min="8" max="10" width="10.7109375" customWidth="1"/>
     <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6564,4 +7842,731 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDF0A5FB-DE8A-C74F-A964-323EA00095A4}">
+  <dimension ref="A1:K18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="32.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
+    <col min="4" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="40" customHeight="1">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="40" customHeight="1">
+      <c r="A2" s="12" t="e" vm="27">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B2" s="5">
+        <f>'[34]Sheet 1'!$AO$115</f>
+        <v>114.61927965594801</v>
+      </c>
+      <c r="C2" s="6">
+        <f>'[34]Sheet 1'!$AO$117</f>
+        <v>-0.66373502418603536</v>
+      </c>
+      <c r="D2" s="6">
+        <f>'[34]Sheet 1'!AM4</f>
+        <v>0.34759551645172948</v>
+      </c>
+      <c r="E2" s="6">
+        <f>'[34]Sheet 1'!$AM$20</f>
+        <v>0.36072951207958304</v>
+      </c>
+      <c r="F2" s="7">
+        <f>'[34]Sheet 1'!$AT$16</f>
+        <v>9.9976925140863973</v>
+      </c>
+      <c r="G2" s="7">
+        <f>'[34]Sheet 1'!$AU$16</f>
+        <v>34.416317733990148</v>
+      </c>
+      <c r="H2" s="6">
+        <f>'[34]Sheet 1'!AS7</f>
+        <v>0.66320000000000001</v>
+      </c>
+      <c r="I2" s="6">
+        <f>'[34]Sheet 1'!AV7</f>
+        <v>0.22484572041856721</v>
+      </c>
+      <c r="J2" s="6">
+        <f>'[34]Sheet 1'!AU13</f>
+        <v>6.2882732764007493E-2</v>
+      </c>
+      <c r="K2" s="8">
+        <f>'[34]Sheet 1'!$AU$101</f>
+        <v>111784200000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="40" customHeight="1">
+      <c r="A3" s="12" t="e" vm="28">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B3" s="5">
+        <f>'[35]Sheet 1'!$V$115</f>
+        <v>243.16631410410545</v>
+      </c>
+      <c r="C3" s="6">
+        <f>'[35]Sheet 1'!$V$117</f>
+        <v>7.6004752883337412E-2</v>
+      </c>
+      <c r="D3" s="6">
+        <f>'[35]Sheet 1'!T4</f>
+        <v>0.21593030491599263</v>
+      </c>
+      <c r="E3" s="6">
+        <f>'[35]Sheet 1'!$T$20</f>
+        <v>0.12399309551208293</v>
+      </c>
+      <c r="F3" s="7">
+        <f>'[35]Sheet 1'!$AA$16</f>
+        <v>15.869447287615149</v>
+      </c>
+      <c r="G3" s="7">
+        <f>'[35]Sheet 1'!$AB$16</f>
+        <v>31.098047736845626</v>
+      </c>
+      <c r="H3" s="6">
+        <f>'[35]Sheet 1'!Z7</f>
+        <v>0.8044</v>
+      </c>
+      <c r="I3" s="6">
+        <f>'[35]Sheet 1'!AC7</f>
+        <v>0.60999658819515523</v>
+      </c>
+      <c r="J3" s="6">
+        <f>'[35]Sheet 1'!AB13</f>
+        <v>0.32418879564370767</v>
+      </c>
+      <c r="K3" s="8">
+        <f>'[35]Sheet 1'!$AB$101</f>
+        <v>465133500000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="40" customHeight="1">
+      <c r="A4" s="12" t="e" vm="29">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B4" s="5">
+        <f>'[30]Sheet 1'!$AD$115</f>
+        <v>338.60998990983916</v>
+      </c>
+      <c r="C4" s="6">
+        <f>'[30]Sheet 1'!$AD$117</f>
+        <v>-0.16347154031859479</v>
+      </c>
+      <c r="D4" s="6">
+        <f>'[30]Sheet 1'!AB4</f>
+        <v>0.15862753660981066</v>
+      </c>
+      <c r="E4" s="6">
+        <f>'[30]Sheet 1'!AB20</f>
+        <v>3.6980525791585839E-2</v>
+      </c>
+      <c r="F4" s="7">
+        <f>'[30]Sheet 1'!AI16</f>
+        <v>8.4120761953520056</v>
+      </c>
+      <c r="G4" s="7">
+        <f>'[30]Sheet 1'!$AJ$16</f>
+        <v>39.078598296369265</v>
+      </c>
+      <c r="H4" s="6">
+        <f>'[30]Sheet 1'!AH7</f>
+        <v>0.52759999999999996</v>
+      </c>
+      <c r="I4" s="6">
+        <f>'[30]Sheet 1'!AK7</f>
+        <v>0.26418087393404821</v>
+      </c>
+      <c r="J4" s="6">
+        <f>'[30]Sheet 1'!AJ13</f>
+        <v>0.13387678195897726</v>
+      </c>
+      <c r="K4" s="8">
+        <f>'[30]Sheet 1'!$AJ$101</f>
+        <v>15510960000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="40" customHeight="1">
+      <c r="A5" s="12" t="e" vm="30">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B5" s="5">
+        <f>'[33]Sheet 1'!$W$115</f>
+        <v>304.30091676100784</v>
+      </c>
+      <c r="C5" s="6">
+        <f>'[33]Sheet 1'!$W$117</f>
+        <v>-0.42977435255128293</v>
+      </c>
+      <c r="D5" s="6">
+        <f>'[33]Sheet 1'!U4</f>
+        <v>0.10034234643345097</v>
+      </c>
+      <c r="E5" s="6">
+        <f>'[33]Sheet 1'!$U$20</f>
+        <v>0.15552034725990227</v>
+      </c>
+      <c r="F5" s="7">
+        <f>'[33]Sheet 1'!$AB$16</f>
+        <v>19.001008628487618</v>
+      </c>
+      <c r="G5" s="7">
+        <f>'[33]Sheet 1'!$AC$16</f>
+        <v>49.077596020092514</v>
+      </c>
+      <c r="H5" s="6">
+        <f>'[33]Sheet 1'!AA7</f>
+        <v>0.77969999999999995</v>
+      </c>
+      <c r="I5" s="6">
+        <f>'[33]Sheet 1'!AD7</f>
+        <v>0.48107843198295114</v>
+      </c>
+      <c r="J5" s="6">
+        <f>'[33]Sheet 1'!AC13</f>
+        <v>0.33217112132371146</v>
+      </c>
+      <c r="K5" s="8">
+        <f>'[33]Sheet 1'!$AC$101</f>
+        <v>42725630000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="40" customHeight="1">
+      <c r="A6" s="12" t="e" vm="31">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B6" s="5">
+        <f>'[29]Sheet 1'!$Z$115</f>
+        <v>277.02893053430296</v>
+      </c>
+      <c r="C6" s="6">
+        <f>'[29]Sheet 1'!$Z$117</f>
+        <v>0.41623092139616036</v>
+      </c>
+      <c r="D6" s="6">
+        <f>'[29]Sheet 1'!X4</f>
+        <v>7.0303004456575113E-2</v>
+      </c>
+      <c r="E6" s="6">
+        <f>'[29]Sheet 1'!X20</f>
+        <v>2.2978549956692351E-2</v>
+      </c>
+      <c r="F6" s="7">
+        <f>'[29]Sheet 1'!AE16</f>
+        <v>13.982792764075388</v>
+      </c>
+      <c r="G6" s="7">
+        <f>'[29]Sheet 1'!$AF$16</f>
+        <v>26.081467855815681</v>
+      </c>
+      <c r="H6" s="6">
+        <f>'[29]Sheet 1'!AD7</f>
+        <v>0.85</v>
+      </c>
+      <c r="I6" s="6">
+        <f>'[29]Sheet 1'!AG7</f>
+        <v>0.60883770968641671</v>
+      </c>
+      <c r="J6" s="6">
+        <f>'[29]Sheet 1'!AF13</f>
+        <v>9.9478512126819518E-2</v>
+      </c>
+      <c r="K6" s="8">
+        <f>'[29]Sheet 1'!$AF$101</f>
+        <v>70185230000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="40" customHeight="1">
+      <c r="A7" s="12" t="e" vm="32">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B7" s="5">
+        <f>'[31]Sheet 1'!$AN$115</f>
+        <v>363.64699332556165</v>
+      </c>
+      <c r="C7" s="6">
+        <f>'[31]Sheet 1'!$AN$117</f>
+        <v>-0.45919664298271667</v>
+      </c>
+      <c r="D7" s="6">
+        <f>'[31]Sheet 1'!AL4</f>
+        <v>4.6131666737559751E-2</v>
+      </c>
+      <c r="E7" s="6">
+        <f>'[31]Sheet 1'!AL20</f>
+        <v>4.0671756745220167E-2</v>
+      </c>
+      <c r="F7" s="7">
+        <f>'[31]Sheet 1'!AS16</f>
+        <v>12.2812302598619</v>
+      </c>
+      <c r="G7" s="7">
+        <f>'[31]Sheet 1'!$AT16</f>
+        <v>45.281695985179674</v>
+      </c>
+      <c r="H7" s="6">
+        <f>'[31]Sheet 1'!AR7</f>
+        <v>0.78059999999999996</v>
+      </c>
+      <c r="I7" s="6">
+        <f>'[31]Sheet 1'!AU7</f>
+        <v>0.36552092182360757</v>
+      </c>
+      <c r="J7" s="6">
+        <f>'[31]Sheet 1'!AT13</f>
+        <v>0.48853670640728536</v>
+      </c>
+      <c r="K7" s="8">
+        <f>'[31]Sheet 1'!$AT$101</f>
+        <v>16914570000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="40" customHeight="1">
+      <c r="A8" s="12" t="e" vm="33">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B8" s="5">
+        <f>'[28]Sheet 1'!$AB$115</f>
+        <v>593.13941771467114</v>
+      </c>
+      <c r="C8" s="6">
+        <f>'[28]Sheet 1'!$AB$117</f>
+        <v>-9.6375049185449146E-2</v>
+      </c>
+      <c r="D8" s="6">
+        <f>'[28]Sheet 1'!Z4</f>
+        <v>-7.7474966449881277E-2</v>
+      </c>
+      <c r="E8" s="6">
+        <f>'[28]Sheet 1'!Z20</f>
+        <v>-0.19460478265991288</v>
+      </c>
+      <c r="F8" s="7">
+        <f>'[28]Sheet 1'!AG16</f>
+        <v>5.5175493761539753</v>
+      </c>
+      <c r="G8" s="7">
+        <f>'[28]Sheet 1'!$AH$16</f>
+        <v>19.04502896871379</v>
+      </c>
+      <c r="H8" s="6">
+        <f>'[28]Sheet 1'!AF7</f>
+        <v>0.49159999999999998</v>
+      </c>
+      <c r="I8" s="6">
+        <f>'[28]Sheet 1'!AI7</f>
+        <v>0.24746824819560231</v>
+      </c>
+      <c r="J8" s="6">
+        <f>'[28]Sheet 1'!AH13</f>
+        <v>0.13786143746414839</v>
+      </c>
+      <c r="K8" s="8">
+        <f>'[28]Sheet 1'!$AH$100</f>
+        <v>98615160000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="40" customHeight="1">
+      <c r="A9" s="12" t="e" vm="34">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B9" s="5">
+        <f>'[32]Sheet 1'!$AC$115</f>
+        <v>137.33486258013255</v>
+      </c>
+      <c r="C9" s="6">
+        <f>'[32]Sheet 1'!$AC$117</f>
+        <v>-0.54010159205635078</v>
+      </c>
+      <c r="D9" s="6">
+        <f>'[32]Sheet 1'!AA4</f>
+        <v>-0.12061756191701511</v>
+      </c>
+      <c r="E9" s="6">
+        <f>'[32]Sheet 1'!AA20</f>
+        <v>-0.41394335511982572</v>
+      </c>
+      <c r="F9" s="7">
+        <f>'[32]Sheet 1'!AH16</f>
+        <v>10.00873811265545</v>
+      </c>
+      <c r="G9" s="7">
+        <f>'[32]Sheet 1'!AI16</f>
+        <v>39.83098981077147</v>
+      </c>
+      <c r="H9" s="6">
+        <f>'[32]Sheet 1'!AG7</f>
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="I9" s="6">
+        <f>'[32]Sheet 1'!AJ7</f>
+        <v>0.26956839795171911</v>
+      </c>
+      <c r="J9" s="6">
+        <f>'[32]Sheet 1'!AI13</f>
+        <v>0.18137160470044308</v>
+      </c>
+      <c r="K9" s="8">
+        <f>'[32]Sheet 1'!AI101</f>
+        <v>54727780000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="40" customHeight="1">
+      <c r="A10" s="12" t="e" vm="35">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B10" s="5">
+        <f>'[27]Sheet 1'!$AL$115</f>
+        <v>338.34949429784706</v>
+      </c>
+      <c r="C10" s="6">
+        <f>'[27]Sheet 1'!$AL$117</f>
+        <v>8.2683735873562592E-2</v>
+      </c>
+      <c r="D10" s="6">
+        <f>'[27]Sheet 1'!AJ4</f>
+        <v>-0.14817164642055514</v>
+      </c>
+      <c r="E10" s="6">
+        <f>'[27]Sheet 1'!$AJ$20</f>
+        <v>-1.0176404064859355</v>
+      </c>
+      <c r="F10" s="7">
+        <f>'[27]Sheet 1'!$AQ$16</f>
+        <v>2.2769253431935623</v>
+      </c>
+      <c r="G10" s="7">
+        <f>'[27]Sheet 1'!$AR$16</f>
+        <v>-30.143043078136639</v>
+      </c>
+      <c r="H10" s="6" t="str">
+        <f>'[27]Sheet 1'!AP7</f>
+        <v>- -</v>
+      </c>
+      <c r="I10" s="6">
+        <f>'[27]Sheet 1'!AS7</f>
+        <v>7.2031752231958138E-2</v>
+      </c>
+      <c r="J10" s="6">
+        <f>'[27]Sheet 1'!AR13</f>
+        <v>-5.3649750927818686E-2</v>
+      </c>
+      <c r="K10" s="8">
+        <f>'[27]Sheet 1'!$AR$101</f>
+        <v>687834100000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="40" customHeight="1">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="8"/>
+    </row>
+    <row r="12" spans="1:11" ht="40" customHeight="1">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="8"/>
+    </row>
+    <row r="13" spans="1:11" ht="40" customHeight="1">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="8"/>
+    </row>
+    <row r="14" spans="1:11" ht="40" customHeight="1">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="8"/>
+    </row>
+    <row r="15" spans="1:11" ht="40" customHeight="1">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="8"/>
+    </row>
+    <row r="16" spans="1:11" ht="40" customHeight="1">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="8"/>
+    </row>
+    <row r="17" spans="8:11" ht="19">
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="8"/>
+    </row>
+    <row r="18" spans="8:11" ht="19">
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="8"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K20">
+    <sortCondition descending="1" ref="D1:D20"/>
+  </sortState>
+  <conditionalFormatting sqref="H11:H18">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11:I18">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J11:J18">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C10">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F10">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D10">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D10">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H10">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I10">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J10">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C10">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E10">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G10">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="A10" r:id="rId1" display="Financials/Berkshire Hathaway.xlsx" xr:uid="{3D5BDD58-8DB7-6F4C-A0C5-DE6286164E2E}"/>
+    <hyperlink ref="A8" r:id="rId2" display="Financials/BlackRock.xlsx" xr:uid="{8C86BB21-B612-B247-8BF0-50D45838B570}"/>
+    <hyperlink ref="A6" r:id="rId3" display="Financials/CME Group.xlsx" xr:uid="{ABDD2171-E931-9A4F-B6BB-DC61743CB1E8}"/>
+    <hyperlink ref="A4" r:id="rId4" display="Financials/FactSet Research Systems.xlsx" xr:uid="{812E59AE-E380-8143-9851-E88C41B1F668}"/>
+    <hyperlink ref="A7" r:id="rId5" display="Financials/Fair Isaac Corporation.xlsx" xr:uid="{DCDBC375-9F08-4A44-8271-C53C499165FD}"/>
+    <hyperlink ref="A9" r:id="rId6" display="Financials/Moodys.xlsx" xr:uid="{740A53AE-9318-2349-BFDF-189F69226EC5}"/>
+    <hyperlink ref="A5" r:id="rId7" display="Financials/MSCI.xlsx" xr:uid="{BEF95854-C8D9-5241-903F-4A9E0075CC26}"/>
+    <hyperlink ref="A2" r:id="rId8" display="Financials/S&amp;P Global.xlsx" xr:uid="{78E65CA9-1EDD-7B45-AC3F-3F8301AA801B}"/>
+    <hyperlink ref="A3" r:id="rId9" display="Financials/Visa.xlsx" xr:uid="{9BB27200-6266-5B4D-90A5-A83B934B20F3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>